<commit_message>
Update mistake in economy report
</commit_message>
<xml_diff>
--- a/dp/economy/ECONOMY_BOOK_KOZYAKOV.xlsx
+++ b/dp/economy/ECONOMY_BOOK_KOZYAKOV.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="27870" windowHeight="13020"/>
+    <workbookView xWindow="4650" yWindow="0" windowWidth="27870" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="160">
   <si>
     <t>Часовая ставка руководителя</t>
   </si>
@@ -527,6 +527,9 @@
   </si>
   <si>
     <t>Прибыль в 2021</t>
+  </si>
+  <si>
+    <t>Сумм</t>
   </si>
 </sst>
 </file>
@@ -1081,8 +1084,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A20:C113" totalsRowShown="0">
-  <autoFilter ref="A20:C113"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A20:C114" totalsRowShown="0">
+  <autoFilter ref="A20:C114"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Сокращение" dataDxfId="2"/>
     <tableColumn id="2" name="Имя" dataDxfId="1"/>
@@ -1355,10 +1358,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H113"/>
+  <dimension ref="A1:H114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F99" sqref="F99"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1848,7 +1851,7 @@
         <v>49</v>
       </c>
       <c r="C30" s="26">
-        <v>7.0000000000000007E-2</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1874,779 +1877,784 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="19"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="29"/>
+      <c r="A33" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="B33" s="16"/>
+      <c r="C33" s="26">
+        <f>SUM(C29:C32)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="15" t="s">
+      <c r="A34" s="19"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="29"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B35" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="C34" s="30">
+      <c r="C35" s="30">
         <f>C29 * C27</f>
         <v>24.882227999999998</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="B35" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="C35" s="30">
-        <f>C30 * C27</f>
-        <v>19.352844000000001</v>
-      </c>
-    </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" s="30">
+        <f>C30 * C27</f>
+        <v>38.705688000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="B36" s="16" t="s">
+      <c r="B37" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="C36" s="30">
+      <c r="C37" s="30">
         <f>C31 * C27</f>
         <v>168.64621199999999</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="17" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="B37" s="18" t="s">
+      <c r="B38" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="C37" s="33">
+      <c r="C38" s="33">
         <f>C32 * C27</f>
         <v>44.235072000000002</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="15"/>
-      <c r="B38" s="16"/>
-      <c r="C38" s="30"/>
-    </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="15" t="s">
+      <c r="A39" s="15"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="30"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="B39" s="16" t="s">
+      <c r="B40" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="C39" s="30">
-        <f>SUM(C34:C37)</f>
-        <v>257.116356</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="17"/>
-      <c r="B40" s="18"/>
-      <c r="C40" s="27"/>
+      <c r="C40" s="30">
+        <f>SUM(C35:C38)</f>
+        <v>276.4692</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="15" t="s">
+      <c r="A41" s="17"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="27"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="B41" s="16" t="s">
+      <c r="B42" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="C41" s="32">
+      <c r="C42" s="32">
         <f>365-4-112-24</f>
         <v>225</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="B42" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="C42" s="26">
-        <v>0.5</v>
-      </c>
-    </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C43" s="26">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="B43" s="16" t="s">
+      <c r="B44" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="C43" s="30">
-        <f>C39 / (C42 * C41)</f>
-        <v>2.28547872</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="34"/>
-      <c r="B44" s="35"/>
-      <c r="C44" s="36"/>
+      <c r="C44" s="30">
+        <f>C40 / (C43 * C42)</f>
+        <v>2.4575040000000001</v>
+      </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="15"/>
-      <c r="B45" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="C45" s="26">
-        <v>1</v>
-      </c>
+      <c r="A45" s="34"/>
+      <c r="B45" s="35"/>
+      <c r="C45" s="36"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="15"/>
       <c r="B46" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C46" s="26">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="15"/>
       <c r="B47" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C47" s="26">
-        <v>67</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="15"/>
       <c r="B48" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C48" s="26">
-        <v>95</v>
+        <v>76</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="15"/>
-      <c r="B49" s="16"/>
-      <c r="C49" s="26"/>
+      <c r="B49" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C49" s="26">
+        <v>100</v>
+      </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="15"/>
-      <c r="B50" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="C50" s="32">
-        <f>C45 * (C47 * G3)</f>
-        <v>1876</v>
-      </c>
+      <c r="B50" s="16"/>
+      <c r="C50" s="26"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="15"/>
       <c r="B51" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C51" s="32">
-        <f>C46 * (C48 * G6)</f>
-        <v>3800</v>
+        <f>C46 * (C48 * G3)</f>
+        <v>2128</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="15"/>
       <c r="B52" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C52" s="32">
-        <f>C50 + C51</f>
-        <v>5676</v>
+        <f>C47 * (C49 * G6)</f>
+        <v>4000</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="15"/>
-      <c r="B53" s="16"/>
-      <c r="C53" s="32"/>
+      <c r="B53" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C53" s="32">
+        <f>C51 + C52</f>
+        <v>6128</v>
+      </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="15" t="s">
+      <c r="A54" s="15"/>
+      <c r="B54" s="16"/>
+      <c r="C54" s="32"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="B54" s="16" t="s">
+      <c r="B55" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="C54" s="32">
-        <f>C52 + (G8 * C52)</f>
-        <v>8514</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="34" t="s">
+      <c r="C55" s="32">
+        <f>C53 + (G8 * C53)</f>
+        <v>9192</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="B55" s="35" t="s">
+      <c r="B56" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="C55" s="37">
-        <f>C54 * G9</f>
-        <v>851.40000000000009</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="39"/>
-      <c r="B56" s="40"/>
-      <c r="C56" s="41"/>
+      <c r="C56" s="37">
+        <f>C55 * G9</f>
+        <v>919.2</v>
+      </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="15" t="s">
+      <c r="A57" s="39"/>
+      <c r="B57" s="40"/>
+      <c r="C57" s="41"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="16" t="s">
+      <c r="B58" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="C57" s="32">
+      <c r="C58" s="32">
         <f>G11 + G12</f>
         <v>0.34600000000000003</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="17" t="s">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="B58" s="18" t="s">
+      <c r="B59" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="C58" s="43">
-        <f>(C54 + C55) * C57</f>
-        <v>3240.4284000000002</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="19"/>
-      <c r="B59" s="20"/>
-      <c r="C59" s="29"/>
-    </row>
-    <row r="60" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="15" t="s">
+      <c r="C59" s="43">
+        <f>(C55 + C56) * C58</f>
+        <v>3498.4752000000008</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="19"/>
+      <c r="B60" s="20"/>
+      <c r="C60" s="29"/>
+    </row>
+    <row r="61" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="B60" s="16" t="s">
+      <c r="B61" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="C60" s="26">
+      <c r="C61" s="26">
         <v>0.12</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="15" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="B61" s="16" t="s">
+      <c r="B62" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="C61" s="32">
-        <f>G16 * C18 * C60</f>
+      <c r="C62" s="32">
+        <f>G16 * C18 * C61</f>
         <v>2150.4</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="17" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="B62" s="18" t="s">
+      <c r="B63" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C62" s="38">
-        <f>C54 * G17</f>
-        <v>9365.4000000000015</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="19"/>
-      <c r="B63" s="20"/>
-      <c r="C63" s="29"/>
+      <c r="C63" s="38">
+        <f>C55 * G17</f>
+        <v>10111.200000000001</v>
+      </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="15" t="s">
+      <c r="A64" s="19"/>
+      <c r="B64" s="20"/>
+      <c r="C64" s="29"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="B64" s="16" t="s">
+      <c r="B65" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="C64" s="42">
-        <f>C54 + C55 + C58 + C61 + C62</f>
-        <v>24121.628400000001</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A65" s="15" t="s">
+      <c r="C65" s="42">
+        <f>C55 + C56 + C59 + C62 + C63</f>
+        <v>25871.275200000004</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A66" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="B65" s="16" t="s">
+      <c r="B66" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="C65" s="26">
+      <c r="C66" s="26">
         <v>0.05</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="15" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="B66" s="16" t="s">
+      <c r="B67" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="C66" s="42">
-        <f>C64 * C65</f>
-        <v>1206.0814200000002</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A67" s="17" t="s">
+      <c r="C67" s="42">
+        <f>C65 * C66</f>
+        <v>1293.5637600000002</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="B67" s="18" t="s">
+      <c r="B68" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="C67" s="43">
-        <f>C64 + C66</f>
-        <v>25327.70982</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="19"/>
-      <c r="B68" s="19"/>
-      <c r="C68" s="29"/>
+      <c r="C68" s="43">
+        <f>C65 + C67</f>
+        <v>27164.838960000005</v>
+      </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="B69" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="C69" s="42">
-        <f>C67 * G19</f>
-        <v>3799.156473</v>
-      </c>
+      <c r="A69" s="19"/>
+      <c r="B69" s="19"/>
+      <c r="C69" s="29"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="B70" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C70" s="42">
+        <f>C68 * G19</f>
+        <v>4074.7258440000005</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="B70" s="16" t="s">
+      <c r="B71" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="C70" s="42">
-        <f>(C67 + C69) * G13</f>
-        <v>5825.3732586000006</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="17" t="s">
+      <c r="C71" s="42">
+        <f>(C68 + C70) * G13</f>
+        <v>6247.9129608000012</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="B71" s="18" t="s">
+      <c r="B72" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="C71" s="43">
-        <f>C67 + C69 + C70</f>
-        <v>34952.239551599996</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="44"/>
-      <c r="B72" s="45"/>
-      <c r="C72" s="46"/>
-    </row>
-    <row r="73" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" s="15" t="s">
+      <c r="C72" s="43">
+        <f>C68 + C70 + C71</f>
+        <v>37487.477764800009</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="44"/>
+      <c r="B73" s="45"/>
+      <c r="C73" s="46"/>
+    </row>
+    <row r="74" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="B73" s="16" t="s">
+      <c r="B74" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="C73" s="26">
+      <c r="C74" s="26">
         <v>0.1</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="15" t="s">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="B74" s="16" t="s">
+      <c r="B75" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="C74" s="42">
-        <f>C67 * C73</f>
-        <v>2532.770982</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="34" t="s">
+      <c r="C75" s="42">
+        <f>C68 * C74</f>
+        <v>2716.4838960000006</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="B75" s="35" t="s">
+      <c r="B76" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="C75" s="47">
-        <f>C71 + C74</f>
-        <v>37485.010533599998</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="39"/>
-      <c r="B76" s="40"/>
-      <c r="C76" s="48"/>
+      <c r="C76" s="47">
+        <f>C72 + C75</f>
+        <v>40203.961660800007</v>
+      </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="B77" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="C77" s="26">
-        <v>5.5</v>
-      </c>
+      <c r="A77" s="39"/>
+      <c r="B77" s="40"/>
+      <c r="C77" s="48"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="15" t="s">
-        <v>41</v>
+        <v>111</v>
       </c>
       <c r="B78" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C78" s="26">
-        <v>3.5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="15" t="s">
-        <v>114</v>
+        <v>41</v>
       </c>
       <c r="B79" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C79" s="26">
-        <v>8</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="B80" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="C80" s="26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="B80" s="16" t="s">
+      <c r="B81" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="C80" s="26">
+      <c r="C81" s="26">
         <v>22</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="B81" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="C81" s="32">
-        <f>(G6 * C80) * (C77 - C78) / C79 / C80 * (1 + G8)</f>
-        <v>7.5</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="B82" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="C82" s="42">
+        <f>(G6 * C81) * (C78 - C79) / C80 / C81 * (1 + G8)</f>
+        <v>5.625</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A83" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="B82" s="16" t="s">
+      <c r="B83" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="C82" s="32">
-        <f>C81 * G9</f>
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="15"/>
-      <c r="B83" s="16" t="s">
+      <c r="C83" s="42">
+        <f>C82 * G9</f>
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="15"/>
+      <c r="B84" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="C83" s="26">
-        <v>1700</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="15" t="s">
+      <c r="C84" s="26">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A85" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="B84" s="16" t="s">
+      <c r="B85" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="C84" s="32">
-        <f>(C81 + C82) * C83</f>
-        <v>14025</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A85" s="34" t="s">
+      <c r="C85" s="32">
+        <f>(C82 + C83) * C84</f>
+        <v>11756.25</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A86" s="34" t="s">
         <v>125</v>
       </c>
-      <c r="B85" s="35" t="s">
+      <c r="B86" s="35" t="s">
         <v>126</v>
       </c>
-      <c r="C85" s="37">
-        <f>C84 * C57</f>
-        <v>4852.6500000000005</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="39"/>
-      <c r="B86" s="40"/>
-      <c r="C86" s="48"/>
-    </row>
-    <row r="87" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A87" s="15" t="s">
+      <c r="C86" s="47">
+        <f>C85 * C58</f>
+        <v>4067.6625000000004</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="39"/>
+      <c r="B87" s="40"/>
+      <c r="C87" s="48"/>
+    </row>
+    <row r="88" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A88" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="B87" s="16" t="s">
+      <c r="B88" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="C87" s="32">
-        <f>G16 * (C77 - C78)</f>
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A88" s="15" t="s">
+      <c r="C88" s="32">
+        <f>G16 * (C78 - C79)</f>
+        <v>1.2000000000000002</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A89" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="B88" s="16" t="s">
+      <c r="B89" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="C88" s="32">
-        <f>C87 * C83</f>
-        <v>2720</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="B89" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="C89" s="26">
-        <v>0.14000000000000001</v>
+      <c r="C89" s="32">
+        <f>C88 * C84</f>
+        <v>2280.0000000000005</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="15" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B90" s="16" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C90" s="26">
-        <v>0.12</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B91" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="C91" s="26">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="B91" s="16" t="s">
+      <c r="B92" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="C91" s="32">
-        <f>C89 - C90</f>
+      <c r="C92" s="32">
+        <f>C90 - C91</f>
         <v>2.0000000000000018E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A92" s="15" t="s">
+    <row r="93" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A93" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="B92" s="16" t="s">
+      <c r="B93" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="C92" s="32">
-        <f>C91 * C83</f>
-        <v>34.000000000000028</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="34" t="s">
+      <c r="C93" s="32">
+        <f>C92 * C84</f>
+        <v>38.000000000000036</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="B93" s="35" t="s">
+      <c r="B94" s="35" t="s">
         <v>139</v>
       </c>
-      <c r="C93" s="37">
-        <f>C84 + C85 + C88 + C92</f>
-        <v>21631.65</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="39"/>
-      <c r="B94" s="40"/>
-      <c r="C94" s="48"/>
+      <c r="C94" s="47">
+        <f>C85 + C86 + C89 + C93</f>
+        <v>18141.912500000002</v>
+      </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="B95" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="C95" s="42">
-        <f>C93 - (C93 * G14)</f>
-        <v>17737.953000000001</v>
-      </c>
+      <c r="A95" s="39"/>
+      <c r="B95" s="40"/>
+      <c r="C95" s="48"/>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="B96" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="C96" s="42">
+        <f>C94 - (C94 * G14)</f>
+        <v>14876.368250000001</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="B96" s="16" t="s">
+      <c r="B97" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="C96" s="42">
+      <c r="C97" s="42">
         <f>(1 + G21)^(1 - 1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="15" t="s">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="B97" s="16" t="s">
+      <c r="B98" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="C97" s="42">
+      <c r="C98" s="42">
         <f>(1 + G21)^(1 - 2)</f>
         <v>0.90497737556561086</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="15" t="s">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="B98" s="16" t="s">
+      <c r="B99" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="C98" s="42">
+      <c r="C99" s="42">
         <f>(1 + G21)^(1 - 3)</f>
         <v>0.81898405028562071</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="15" t="s">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="B99" s="16" t="s">
+      <c r="B100" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="C99" s="42">
+      <c r="C100" s="42">
         <f>(1 + G21)^(1 - 4)</f>
         <v>0.74116203645757528</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="15"/>
-      <c r="B100" s="16"/>
-      <c r="C100" s="32"/>
-    </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="15" t="s">
-        <v>151</v>
-      </c>
+      <c r="A101" s="15"/>
       <c r="B101" s="16"/>
-      <c r="C101" s="42">
-        <f>$C95 * C96</f>
-        <v>17737.953000000001</v>
-      </c>
+      <c r="C101" s="32"/>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B102" s="16"/>
       <c r="C102" s="42">
-        <f>C95 * C97</f>
-        <v>16052.446153846155</v>
+        <f>$C96 * C97</f>
+        <v>14876.368250000001</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B103" s="16"/>
       <c r="C103" s="42">
-        <f>C95 * C98</f>
-        <v>14527.100591715978</v>
+        <f>C96 * C98</f>
+        <v>13462.776696832581</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B104" s="16"/>
       <c r="C104" s="42">
-        <f>C95 * C99</f>
-        <v>13146.697368068757</v>
+        <f>C96 * C99</f>
+        <v>12183.508322925412</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="15"/>
+      <c r="A105" s="15" t="s">
+        <v>154</v>
+      </c>
       <c r="B105" s="16"/>
-      <c r="C105" s="32"/>
+      <c r="C105" s="42">
+        <f>C96 * C100</f>
+        <v>11025.799387262816</v>
+      </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="15" t="s">
+      <c r="A106" s="15"/>
+      <c r="B106" s="16"/>
+      <c r="C106" s="32"/>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="B106" s="16"/>
-      <c r="C106" s="42">
-        <f>C95 - C75</f>
-        <v>-19747.057533599997</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="15"/>
       <c r="B107" s="16"/>
-      <c r="C107" s="26"/>
+      <c r="C107" s="42">
+        <f>C96 - C76</f>
+        <v>-25327.593410800007</v>
+      </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="15"/>
-      <c r="B108" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C108" s="42">
-        <f>C106 + C102</f>
-        <v>-3694.6113797538419</v>
-      </c>
+      <c r="B108" s="16"/>
+      <c r="C108" s="26"/>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="15"/>
       <c r="B109" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C109" s="42">
-        <f>C108 + C103</f>
-        <v>10832.489211962136</v>
+        <f>C107 + C103</f>
+        <v>-11864.816713967426</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="15"/>
       <c r="B110" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C110" s="42">
         <f>C109 + C104</f>
-        <v>23979.186580030895</v>
+        <v>318.69160895798632</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="15"/>
-      <c r="B111" s="16"/>
-      <c r="C111" s="26"/>
+      <c r="B111" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="C111" s="42">
+        <f>C110 + C105</f>
+        <v>11344.490996220802</v>
+      </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="15"/>
@@ -2657,6 +2665,11 @@
       <c r="A113" s="15"/>
       <c r="B113" s="16"/>
       <c r="C113" s="26"/>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="15"/>
+      <c r="B114" s="16"/>
+      <c r="C114" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>